<commit_message>
update capability statemetn and fix links
</commit_message>
<xml_diff>
--- a/source/resources/source-data/capstatements-spreadsheets/alert-initiator.xlsx
+++ b/source/resources/source-data/capstatements-spreadsheets/alert-initiator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-Alerts\source\resources\source-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-Notifications\source\resources\source-data\capstatements-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840E8D60-0445-4777-9CFB-7F1C8D5311EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DAF0A1-FC36-4E69-A704-16119155DEB9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-465" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="138">
   <si>
     <t>Element</t>
   </si>
@@ -132,9 +132,6 @@
     <t>referencePolicy</t>
   </si>
   <si>
-    <t>resolves</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -270,39 +267,12 @@
     <t>should_include</t>
   </si>
   <si>
-    <t>conf_Device</t>
-  </si>
-  <si>
-    <t>conf_DiagnosticReport</t>
-  </si>
-  <si>
-    <t>conf_DocumentReference</t>
-  </si>
-  <si>
     <t>conf_Encounter</t>
   </si>
   <si>
-    <t>conf_Goal</t>
-  </si>
-  <si>
-    <t>conf_Immunization</t>
-  </si>
-  <si>
     <t>conf_Location</t>
   </si>
   <si>
-    <t>conf_Medication</t>
-  </si>
-  <si>
-    <t>conf_MedicationRequest</t>
-  </si>
-  <si>
-    <t>conf_MedicationStatement</t>
-  </si>
-  <si>
-    <t>conf_Observation</t>
-  </si>
-  <si>
     <t>conf_Organization</t>
   </si>
   <si>
@@ -315,9 +285,6 @@
     <t>conf_PractitionerRole</t>
   </si>
   <si>
-    <t>conf_Procedure</t>
-  </si>
-  <si>
     <t>conditionalCreate</t>
   </si>
   <si>
@@ -360,89 +327,22 @@
     <t>referencePolicy_conf</t>
   </si>
   <si>
-    <t>doc_DiagnosticReport</t>
-  </si>
-  <si>
-    <t>Communication</t>
-  </si>
-  <si>
-    <t>Da Vinci Alerts Communication Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-alerts/StructureDefinition/alerts-communication</t>
-  </si>
-  <si>
     <t>Coverage</t>
   </si>
   <si>
-    <t>conf_Communication</t>
-  </si>
-  <si>
     <t>conf_Coverage</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core-3.0.0</t>
-  </si>
-  <si>
     <t xml:space="preserve"> US Core Implementation Guide STU 3</t>
   </si>
   <si>
-    <t>transaction</t>
-  </si>
-  <si>
-    <t>batch</t>
-  </si>
-  <si>
-    <t>search-system</t>
-  </si>
-  <si>
-    <t>history-system</t>
-  </si>
-  <si>
     <t>doc</t>
   </si>
   <si>
-    <t>Da Vinci Alerts Bundle Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-alerts/StructureDefinition/alerts-bundle</t>
-  </si>
-  <si>
     <t>Bundle</t>
   </si>
   <si>
-    <t>notify</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-alerts/OperationDefinition/notify</t>
-  </si>
-  <si>
-    <t>A server **SHALL** be capable of invoking the $notify operation to alert the Alert Recipient or Alert Intermediary of a patient event.
-`GET [base]/Communication/$notify`</t>
-  </si>
-  <si>
     <t>conf_Bundle</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/StructureDefinition/hrex-coverage</t>
-  </si>
-  <si>
-    <t>HRex Coverage Profile</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-alerts/ImplementationGuide/hl7.fhir.us.davinci-alerts-0.1.0</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-alerts/StructureDefinition/alerts-endpoint</t>
-  </si>
-  <si>
-    <t>Da Vinci Alerts Endpoint Profile</t>
-  </si>
-  <si>
-    <t>Endpoint</t>
-  </si>
-  <si>
-    <t>conf_Endpoint</t>
   </si>
   <si>
     <t>client</t>
@@ -453,20 +353,149 @@
 </t>
   </si>
   <si>
-    <t>alert-initiator</t>
-  </si>
-  <si>
-    <t>This CapabilityStatement describes the expected capabilities of a client that is capable of sending an alert by initiating the Da Vinci Notify Operation.</t>
-  </si>
-  <si>
-    <t>The Da Vinci Alerts $notify Initiator **SHALL**:
-1. Support at least one use case defined in this Guide and listed in the [Scenarios](index.html#scenarios) Section.
+    <t>version</t>
+  </si>
+  <si>
+    <t>0.1.0</t>
+  </si>
+  <si>
+    <t>fhirVersion</t>
+  </si>
+  <si>
+    <t>4.0.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core|3.1.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/ImplementationGuide/hl7.fhir.us.davinci-notifications|0.1.0</t>
+  </si>
+  <si>
+    <t>This CapabilityStatement describes the expected capabilities of a client that is capable of sending a Da Vinci Unsolicited Notification transacted with the `$process-message` operation.</t>
+  </si>
+  <si>
+    <t>Da Vinci Notifications Bundle Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/notifications-bundle</t>
+  </si>
+  <si>
+    <t>notification-sender</t>
+  </si>
+  <si>
+    <t>The Da Vinci Notification Sender **SHALL**:
+1. Support the admission/discharge use case defined in this Guide.
 1. Implement the RESTful behavior according to the FHIR specification.
-1. Support json source formats for all Da Vinci Alert interactions.
+1. Support json source formats for all Da Vinci Notification interactions.
 1. Declare a CapabilityStatement identifying the scenarios, transactions and profiles supported.
-The Da Vinci Alerts $notify Initiator **SHOULD**:
-1. Support xml source formats for all Da Vinci Alert interactions.
-1. Identify the Da Vinci Alert or US Core profiles supported as part of the FHIR `meta.profile` attribute for each instance.</t>
+The Da Vinci Notifications Sender **SHOULD**:
+1. Support xml source formats for all Da Vinci Notification interactions.
+1. Identify the Da Vinci or US Core profiles supported as part of the FHIR `meta.profile` attribute for each instance.</t>
+  </si>
+  <si>
+    <t>Da Vinci Notifications MessageHeader Profile</t>
+  </si>
+  <si>
+    <t>Da Vinci Notifications MessageDefinition Profile</t>
+  </si>
+  <si>
+    <t>Da Vinci Notifications GraphDefinition Profile</t>
+  </si>
+  <si>
+    <t>Da Vinci Admit Notification MessageHeader Profile</t>
+  </si>
+  <si>
+    <t>Da Vinci Discharge Notification MessageHeader Profile</t>
+  </si>
+  <si>
+    <t>Da Vinci Admit/Discharge Notification Condition Profile</t>
+  </si>
+  <si>
+    <t>Da Vinci Admit/Discharge Notification Coverage Profile</t>
+  </si>
+  <si>
+    <t>​Da Vinci Admit/Discharge Notification Encounter Profile</t>
+  </si>
+  <si>
+    <t>MessageHeader</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Encounter</t>
+  </si>
+  <si>
+    <t>MessageDefinition</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/notifications-messageheader</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/notifications-messagedefinition</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/notifications-graphdefinition</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-notification-messageheader</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/discharge-notification-messageheader</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-discharge-notification-condition</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-discharge-notification-encounter</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-discharge-notification-coverage</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Practitioner</t>
+  </si>
+  <si>
+    <t>PractitionerRole</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>conf_MessageHeader</t>
+  </si>
+  <si>
+    <t>conf_GraphDefinition</t>
+  </si>
+  <si>
+    <t>conf_MessageDefinition</t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/OperationDefinition/MessageHeader-process-message</t>
+  </si>
+  <si>
+    <t>The Sender SHALL notify the Recipient or Intermediary using the $process-message operation.</t>
+  </si>
+  <si>
+    <t>GraphDefinition</t>
+  </si>
+  <si>
+    <t>conf_Condition</t>
+  </si>
+  <si>
+    <t>Required resource type to carry information regarding admission and discharge event in the Da Vinci Notification message bundle</t>
+  </si>
+  <si>
+    <t>process-message</t>
   </si>
 </sst>
 </file>
@@ -940,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -965,47 +994,63 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="105" customHeight="1">
-      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1">
+      <c r="A3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="1" customFormat="1">
+      <c r="A4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="105" customHeight="1">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="B5" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B6" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="351.75" customHeight="1">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="207.75" customHeight="1">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="103.5" customHeight="1">
-      <c r="A7" t="s">
+      <c r="B8" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="103.5" customHeight="1">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>124</v>
+      <c r="B9" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1018,7 +1063,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1028,10 +1073,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>14</v>
@@ -1039,10 +1084,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
@@ -1058,7 +1103,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1085,75 +1130,135 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="B10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6">
@@ -1217,7 +1322,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1248,118 +1353,182 @@
         <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="H1" t="s">
         <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="R1" t="s">
         <v>18</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="T1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="V1" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickTop="1">
-      <c r="A2" t="s">
-        <v>99</v>
+      <c r="A2" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:23">
-      <c r="A3" t="s">
-        <v>96</v>
+      <c r="A3" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" t="s">
-        <v>111</v>
+      <c r="A4" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:23" ht="45">
+      <c r="A6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="R5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>55</v>
+      <c r="C6" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="45">
+      <c r="A7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="45">
+      <c r="A8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="45">
+      <c r="A9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="45">
+      <c r="A10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="45">
+      <c r="A11" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="45">
+      <c r="A12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="45">
+      <c r="A13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="20:23" ht="18">
@@ -1381,12 +1550,12 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="77.42578125" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
@@ -1395,36 +1564,36 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
       </c>
       <c r="C1" t="s">
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60.75" thickBot="1">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1">
       <c r="A2" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>113</v>
+        <v>137</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>132</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1432,679 +1601,250 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S15" sqref="S15"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="58.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
-    <col min="19" max="19" width="37.42578125" customWidth="1"/>
-    <col min="22" max="22" width="13" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="R1" t="s">
-        <v>80</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>12</v>
-      </c>
-      <c r="R3" t="s">
-        <v>12</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>12</v>
-      </c>
-      <c r="R4" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
-      <c r="A5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L5" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" t="s">
-        <v>55</v>
-      </c>
-      <c r="P5" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>55</v>
-      </c>
-      <c r="R5" t="s">
-        <v>55</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
-      <c r="A6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R6" t="s">
-        <v>27</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N7" t="s">
-        <v>27</v>
-      </c>
-      <c r="O7" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>27</v>
-      </c>
-      <c r="R7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L8" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P8" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>27</v>
-      </c>
-      <c r="R8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" t="s">
-        <v>55</v>
-      </c>
-      <c r="H9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I9" t="s">
-        <v>55</v>
-      </c>
-      <c r="J9" t="s">
-        <v>55</v>
-      </c>
-      <c r="K9" t="s">
-        <v>55</v>
-      </c>
-      <c r="L9" t="s">
-        <v>55</v>
-      </c>
-      <c r="M9" t="s">
-        <v>55</v>
-      </c>
-      <c r="N9" t="s">
-        <v>55</v>
-      </c>
-      <c r="O9" t="s">
-        <v>55</v>
-      </c>
-      <c r="P9" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>55</v>
-      </c>
-      <c r="R9" t="s">
-        <v>55</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" t="s">
-        <v>27</v>
-      </c>
-      <c r="M10" t="s">
-        <v>27</v>
-      </c>
-      <c r="N10" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" t="s">
-        <v>27</v>
-      </c>
-      <c r="P10" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>27</v>
-      </c>
-      <c r="R10" t="s">
-        <v>27</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>27</v>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2115,10 +1855,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D418CE29-40DC-476E-89CD-A42CEC26847E}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2129,49 +1869,19 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1">
-      <c r="A2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="C2" s="2"/>
       <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2218,88 +1928,88 @@
   <sheetData>
     <row r="1" spans="1:28" ht="18.95" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="W1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="U1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="Z1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="AA1" s="13" t="s">
-        <v>53</v>
-      </c>
       <c r="AB1" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="1" customFormat="1" ht="18.95" customHeight="1" thickTop="1">
@@ -2829,7 +2539,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AB92" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
-  <sortState ref="A7:AA34">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA34">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2846,7 +2556,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="G61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B79" sqref="B79"/>
+      <selection pane="bottomRight" activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2865,34 +2575,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1">

</xml_diff>

<commit_message>
update to conformance statement
</commit_message>
<xml_diff>
--- a/source/resources/source-data/capstatements-spreadsheets/alert-initiator.xlsx
+++ b/source/resources/source-data/capstatements-spreadsheets/alert-initiator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-Notifications\source\resources\source-data\capstatements-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DAF0A1-FC36-4E69-A704-16119155DEB9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B5AB33-2E1B-4F05-89CD-4C4F0E122FA1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-465" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -383,119 +383,120 @@
     <t>notification-sender</t>
   </si>
   <si>
+    <t>Da Vinci Notifications MessageHeader Profile</t>
+  </si>
+  <si>
+    <t>Da Vinci Notifications MessageDefinition Profile</t>
+  </si>
+  <si>
+    <t>Da Vinci Notifications GraphDefinition Profile</t>
+  </si>
+  <si>
+    <t>Da Vinci Admit Notification MessageHeader Profile</t>
+  </si>
+  <si>
+    <t>Da Vinci Discharge Notification MessageHeader Profile</t>
+  </si>
+  <si>
+    <t>Da Vinci Admit/Discharge Notification Condition Profile</t>
+  </si>
+  <si>
+    <t>Da Vinci Admit/Discharge Notification Coverage Profile</t>
+  </si>
+  <si>
+    <t>​Da Vinci Admit/Discharge Notification Encounter Profile</t>
+  </si>
+  <si>
+    <t>MessageHeader</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Encounter</t>
+  </si>
+  <si>
+    <t>MessageDefinition</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/notifications-messageheader</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/notifications-messagedefinition</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/notifications-graphdefinition</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-notification-messageheader</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/discharge-notification-messageheader</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-discharge-notification-condition</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-discharge-notification-encounter</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-discharge-notification-coverage</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Practitioner</t>
+  </si>
+  <si>
+    <t>PractitionerRole</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>conf_MessageHeader</t>
+  </si>
+  <si>
+    <t>conf_GraphDefinition</t>
+  </si>
+  <si>
+    <t>conf_MessageDefinition</t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/OperationDefinition/MessageHeader-process-message</t>
+  </si>
+  <si>
+    <t>The Sender SHALL notify the Recipient or Intermediary using the $process-message operation.</t>
+  </si>
+  <si>
+    <t>GraphDefinition</t>
+  </si>
+  <si>
+    <t>conf_Condition</t>
+  </si>
+  <si>
+    <t>Required resource type to carry information regarding admission and discharge event in the Da Vinci Notification message bundle</t>
+  </si>
+  <si>
+    <t>process-message</t>
+  </si>
+  <si>
     <t>The Da Vinci Notification Sender **SHALL**:
-1. Support the admission/discharge use case defined in this Guide.
+1. Support the notification framework defined in this Guide.
 1. Implement the RESTful behavior according to the FHIR specification.
 1. Support json source formats for all Da Vinci Notification interactions.
 1. Declare a CapabilityStatement identifying the scenarios, transactions and profiles supported.
 The Da Vinci Notifications Sender **SHOULD**:
+1. Support the admission/discharge use case defined in this Guide.
 1. Support xml source formats for all Da Vinci Notification interactions.
 1. Identify the Da Vinci or US Core profiles supported as part of the FHIR `meta.profile` attribute for each instance.</t>
-  </si>
-  <si>
-    <t>Da Vinci Notifications MessageHeader Profile</t>
-  </si>
-  <si>
-    <t>Da Vinci Notifications MessageDefinition Profile</t>
-  </si>
-  <si>
-    <t>Da Vinci Notifications GraphDefinition Profile</t>
-  </si>
-  <si>
-    <t>Da Vinci Admit Notification MessageHeader Profile</t>
-  </si>
-  <si>
-    <t>Da Vinci Discharge Notification MessageHeader Profile</t>
-  </si>
-  <si>
-    <t>Da Vinci Admit/Discharge Notification Condition Profile</t>
-  </si>
-  <si>
-    <t>Da Vinci Admit/Discharge Notification Coverage Profile</t>
-  </si>
-  <si>
-    <t>​Da Vinci Admit/Discharge Notification Encounter Profile</t>
-  </si>
-  <si>
-    <t>MessageHeader</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t>Encounter</t>
-  </si>
-  <si>
-    <t>MessageDefinition</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/notifications-messageheader</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/notifications-messagedefinition</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/notifications-graphdefinition</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-notification-messageheader</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/discharge-notification-messageheader</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-discharge-notification-condition</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-discharge-notification-encounter</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-discharge-notification-coverage</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
-    <t>Practitioner</t>
-  </si>
-  <si>
-    <t>PractitionerRole</t>
-  </si>
-  <si>
-    <t>Patient</t>
-  </si>
-  <si>
-    <t>conf_MessageHeader</t>
-  </si>
-  <si>
-    <t>conf_GraphDefinition</t>
-  </si>
-  <si>
-    <t>conf_MessageDefinition</t>
-  </si>
-  <si>
-    <t>system</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/OperationDefinition/MessageHeader-process-message</t>
-  </si>
-  <si>
-    <t>The Sender SHALL notify the Recipient or Intermediary using the $process-message operation.</t>
-  </si>
-  <si>
-    <t>GraphDefinition</t>
-  </si>
-  <si>
-    <t>conf_Condition</t>
-  </si>
-  <si>
-    <t>Required resource type to carry information regarding admission and discharge event in the Da Vinci Notification message bundle</t>
-  </si>
-  <si>
-    <t>process-message</t>
   </si>
 </sst>
 </file>
@@ -971,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1042,7 +1043,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="103.5" customHeight="1">
@@ -1130,16 +1131,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -1159,84 +1160,84 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>54</v>
@@ -1248,16 +1249,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -1322,7 +1323,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1412,7 +1413,7 @@
     </row>
     <row r="2" spans="1:23" ht="15.75" thickTop="1">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -1428,7 +1429,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>54</v>
@@ -1436,7 +1437,7 @@
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>54</v>
@@ -1445,13 +1446,13 @@
     </row>
     <row r="6" spans="1:23" ht="45">
       <c r="A6" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="45">
@@ -1459,76 +1460,76 @@
         <v>84</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="45">
       <c r="A8" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="45">
       <c r="A9" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="45">
       <c r="A10" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="45">
       <c r="A11" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="45">
       <c r="A12" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="45">
       <c r="A13" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="20:23" ht="18">
@@ -1581,19 +1582,19 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1">
       <c r="A2" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1631,10 +1632,10 @@
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>85</v>
@@ -1643,10 +1644,10 @@
         <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
FHIR-26274, FHIR-26270, and other
</commit_message>
<xml_diff>
--- a/source/resources/source-data/capstatements-spreadsheets/alert-initiator.xlsx
+++ b/source/resources/source-data/capstatements-spreadsheets/alert-initiator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-Notifications\source\resources\source-data\capstatements-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B5AB33-2E1B-4F05-89CD-4C4F0E122FA1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398C0084-3D34-45DF-A48F-F9E685531CE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-465" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">sp_combos!$B$1:$B$81</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">sps!$A$1:$AB$92</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -368,18 +368,12 @@
     <t>http://hl7.org/fhir/us/core/ImplementationGuide/hl7.fhir.us.core|3.1.0</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/ImplementationGuide/hl7.fhir.us.davinci-notifications|0.1.0</t>
-  </si>
-  <si>
     <t>This CapabilityStatement describes the expected capabilities of a client that is capable of sending a Da Vinci Unsolicited Notification transacted with the `$process-message` operation.</t>
   </si>
   <si>
     <t>Da Vinci Notifications Bundle Profile</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/notifications-bundle</t>
-  </si>
-  <si>
     <t>notification-sender</t>
   </si>
   <si>
@@ -417,30 +411,6 @@
   </si>
   <si>
     <t>MessageDefinition</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/notifications-messageheader</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/notifications-messagedefinition</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/notifications-graphdefinition</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-notification-messageheader</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/discharge-notification-messageheader</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-discharge-notification-condition</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-discharge-notification-encounter</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-notifications/StructureDefinition/admit-discharge-notification-coverage</t>
   </si>
   <si>
     <t>Location</t>
@@ -497,6 +467,36 @@
 1. Support the admission/discharge use case defined in this Guide.
 1. Support xml source formats for all Da Vinci Notification interactions.
 1. Identify the Da Vinci or US Core profiles supported as part of the FHIR `meta.profile` attribute for each instance.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-alerts/ImplementationGuide/hl7.fhir.us.davinci-alerts|0.1.0</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-alerts/StructureDefinition/notifications-messageheader</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-alerts/StructureDefinition/notifications-bundle</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-alerts/StructureDefinition/notifications-messagedefinition</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-alerts/StructureDefinition/notifications-graphdefinition</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-alerts/StructureDefinition/admit-notification-messageheader</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-alerts/StructureDefinition/discharge-notification-messageheader</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-alerts/StructureDefinition/admit-discharge-notification-condition</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-alerts/StructureDefinition/admit-discharge-notification-coverage</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-alerts/StructureDefinition/admit-discharge-notification-encounter</t>
   </si>
 </sst>
 </file>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -995,7 +995,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1">
@@ -1019,7 +1019,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1027,7 +1027,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1043,7 +1043,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="103.5" customHeight="1">
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1131,25 +1131,25 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -1160,84 +1160,84 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>54</v>
@@ -1249,16 +1249,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="2" spans="1:23" ht="15.75" thickTop="1">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>54</v>
@@ -1437,7 +1437,7 @@
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>54</v>
@@ -1446,13 +1446,13 @@
     </row>
     <row r="6" spans="1:23" ht="45">
       <c r="A6" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="45">
@@ -1463,73 +1463,73 @@
         <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="45">
       <c r="A8" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="45">
       <c r="A9" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="45">
       <c r="A10" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="45">
       <c r="A11" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="45">
       <c r="A12" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="45">
       <c r="A13" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="20:23" ht="18">
@@ -1582,19 +1582,19 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1">
       <c r="A2" s="15" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1632,10 +1632,10 @@
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>85</v>
@@ -1644,10 +1644,10 @@
         <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>64</v>

</xml_diff>